<commit_message>
some data for sunrise/set for photoresistor
</commit_message>
<xml_diff>
--- a/Arduino datapoints for photoresistor.xlsx
+++ b/Arduino datapoints for photoresistor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aankit\Desktop\Homework\Engineering code Screenshots\ENGR122\Design project\ENGR122-Design-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B38CC2-76AE-4702-9CFE-D600C7047707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05A11B6-F446-46C1-829A-F160335524FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10740" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -984,7 +984,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="5" spans="1:12" s="15" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
-        <v>43939.348813842589</v>
+        <v>43939.891462662039</v>
       </c>
       <c r="B5" s="36">
-        <v>961</v>
+        <v>3</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -1155,10 +1155,10 @@
     </row>
     <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
-        <v>43939.347841180555</v>
+        <v>43939.890489988429</v>
       </c>
       <c r="B8" s="38">
-        <v>955</v>
+        <v>4</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -1173,10 +1173,10 @@
     </row>
     <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
-        <v>43939.347910682867</v>
+        <v>43939.890559444444</v>
       </c>
       <c r="B9" s="37">
-        <v>955</v>
+        <v>4</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
-        <v>43939.347980138889</v>
+        <v>43939.890628946756</v>
       </c>
       <c r="B10" s="37">
-        <v>956</v>
+        <v>3</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
@@ -1209,10 +1209,10 @@
     </row>
     <row r="11" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
-        <v>43939.348049629632</v>
+        <v>43939.890698425923</v>
       </c>
       <c r="B11" s="37">
-        <v>957</v>
+        <v>4</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -1227,10 +1227,10 @@
     </row>
     <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
-        <v>43939.348119120368</v>
+        <v>43939.890767881945</v>
       </c>
       <c r="B12" s="37">
-        <v>957</v>
+        <v>4</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
-        <v>43939.348188564814</v>
+        <v>43939.890837372688</v>
       </c>
       <c r="B13" s="37">
-        <v>959</v>
+        <v>3</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -1263,10 +1263,10 @@
     </row>
     <row r="14" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
-        <v>43939.348258067126</v>
+        <v>43939.890906828703</v>
       </c>
       <c r="B14" s="37">
-        <v>960</v>
+        <v>3</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -1281,10 +1281,10 @@
     </row>
     <row r="15" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
-        <v>43939.348327523148</v>
+        <v>43939.890976331022</v>
       </c>
       <c r="B15" s="37">
-        <v>959</v>
+        <v>4</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -1299,10 +1299,10 @@
     </row>
     <row r="16" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
-        <v>43939.348397013891</v>
+        <v>43939.891045810182</v>
       </c>
       <c r="B16" s="37">
-        <v>960</v>
+        <v>4</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="17" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
-        <v>43939.348466504627</v>
+        <v>43939.89111527778</v>
       </c>
       <c r="B17" s="37">
-        <v>960</v>
+        <v>3</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -1335,10 +1335,10 @@
     </row>
     <row r="18" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
-        <v>43939.348535960649</v>
+        <v>43939.891184768516</v>
       </c>
       <c r="B18" s="37">
-        <v>962</v>
+        <v>2</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -1353,10 +1353,10 @@
     </row>
     <row r="19" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
-        <v>43939.348605451392</v>
+        <v>43939.891254259259</v>
       </c>
       <c r="B19" s="37">
-        <v>961</v>
+        <v>3</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -1371,10 +1371,10 @@
     </row>
     <row r="20" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
-        <v>43939.348674907407</v>
+        <v>43939.891323703705</v>
       </c>
       <c r="B20" s="37">
-        <v>962</v>
+        <v>3</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
@@ -1389,10 +1389,10 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
-        <v>43939.348744409719</v>
+        <v>43939.891393206017</v>
       </c>
       <c r="B21" s="37">
-        <v>961</v>
+        <v>3</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -1407,10 +1407,10 @@
     </row>
     <row r="22" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
-        <v>43939.348813842589</v>
+        <v>43939.891462662039</v>
       </c>
       <c r="B22" s="35">
-        <v>961</v>
+        <v>3</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>

</xml_diff>